<commit_message>
Revert "added blot comment"
This reverts commit 9c66ac3c9ab15e767e5bc7d2a55f3838c38701a5.
</commit_message>
<xml_diff>
--- a/GreenEdgeTargetProteinSamplePrep.xlsx
+++ b/GreenEdgeTargetProteinSamplePrep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msavoie\Campbell Lab Dropbox\Mireille Savoie\GreenEdgeProtein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F75F732-3E88-40BF-80C1-4DFB57D1EE74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC7E4C9-2C55-4EBD-A689-9399BADE1A93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{45A26B87-A4C7-4FD4-AD9A-0A3352E67DF9}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45A26B87-A4C7-4FD4-AD9A-0A3352E67DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4860" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="349">
   <si>
     <t>P143</t>
   </si>
@@ -1083,15 +1083,6 @@
   <si>
     <t>20200714RbcLblot14c</t>
   </si>
-  <si>
-    <t>20200716RbcLblot15a</t>
-  </si>
-  <si>
-    <t>above std curve</t>
-  </si>
-  <si>
-    <t>Bad blot</t>
-  </si>
 </sst>
 </file>
 
@@ -1579,13 +1570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C7128F-9919-43DF-B835-0087BB6AD32F}">
-  <dimension ref="A1:BB708"/>
+  <dimension ref="A1:BB695"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AD690" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="V660" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH700" sqref="AH700"/>
+      <selection pane="bottomRight" activeCell="AG684" sqref="AG684:AG695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -80256,7 +80247,7 @@
         <v>44014</v>
       </c>
       <c r="G684" s="26">
-        <f t="shared" ref="G684:G708" si="425">$B684/$E684</f>
+        <f t="shared" ref="G684:G695" si="425">$B684/$E684</f>
         <v>4.8340853655680057E-3</v>
       </c>
       <c r="K684" s="47">
@@ -80280,45 +80271,45 @@
         <v>24.91</v>
       </c>
       <c r="T684" s="2">
-        <f t="shared" ref="T684:T708" si="426">$R684*0.1</f>
+        <f t="shared" ref="T684:T695" si="426">$R684*0.1</f>
         <v>3</v>
       </c>
       <c r="U684" s="2">
         <v>2.09</v>
       </c>
       <c r="V684" s="2">
-        <f t="shared" ref="V684:V708" si="427">$R684-($S684+$T684+$U684)</f>
+        <f t="shared" ref="V684:V695" si="427">$R684-($S684+$T684+$U684)</f>
         <v>0</v>
       </c>
       <c r="W684" s="5">
-        <f t="shared" ref="W684:W708" si="428">SUM($S684:$V684)</f>
+        <f t="shared" ref="W684:W695" si="428">SUM($S684:$V684)</f>
         <v>30</v>
       </c>
       <c r="X684" s="22">
         <v>2.4</v>
       </c>
       <c r="Y684" s="2">
-        <f t="shared" ref="Y684:Y708" si="429">$S684*$X684</f>
+        <f t="shared" ref="Y684:Y695" si="429">$S684*$X684</f>
         <v>59.783999999999999</v>
       </c>
       <c r="Z684" s="2">
-        <f t="shared" ref="Z684:Z708" si="430">$T684*$X684</f>
+        <f t="shared" ref="Z684:Z695" si="430">$T684*$X684</f>
         <v>7.1999999999999993</v>
       </c>
       <c r="AA684" s="2">
-        <f t="shared" ref="AA684:AA708" si="431">$U684*$X684</f>
+        <f t="shared" ref="AA684:AA695" si="431">$U684*$X684</f>
         <v>5.0159999999999991</v>
       </c>
       <c r="AB684" s="2">
-        <f t="shared" ref="AB684:AB708" si="432">$V684*$X684</f>
+        <f t="shared" ref="AB684:AB695" si="432">$V684*$X684</f>
         <v>0</v>
       </c>
       <c r="AC684" s="2">
-        <f t="shared" ref="AC684:AC708" si="433">SUM($Y684:$AB684)</f>
+        <f t="shared" ref="AC684:AC695" si="433">SUM($Y684:$AB684)</f>
         <v>72</v>
       </c>
       <c r="AD684" s="13">
-        <f t="shared" ref="AD684:AD708" si="434">$G684*$Y684/$AC684</f>
+        <f t="shared" ref="AD684:AD695" si="434">$G684*$Y684/$AC684</f>
         <v>4.0139022152099676E-3</v>
       </c>
       <c r="AE684" s="44">
@@ -80335,11 +80326,11 @@
         <v>5</v>
       </c>
       <c r="AI684" s="2">
-        <f t="shared" ref="AI684:AI708" si="435">$Y684*($AH684/$AC684)</f>
+        <f t="shared" ref="AI684:AI695" si="435">$Y684*($AH684/$AC684)</f>
         <v>4.1516666666666664</v>
       </c>
       <c r="AJ684" s="3">
-        <f t="shared" ref="AJ684:AJ708" si="436">$AD684*$AH684</f>
+        <f t="shared" ref="AJ684:AJ695" si="436">$AD684*$AH684</f>
         <v>2.0069511076049838E-2</v>
       </c>
       <c r="AK684" s="47">
@@ -80347,9 +80338,6 @@
         <v>9.1336666666666663E-2</v>
       </c>
       <c r="AL684" s="9"/>
-      <c r="AM684" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN684" s="43" t="s">
         <v>334</v>
       </c>
@@ -80483,9 +80471,6 @@
         <v>0.26985833333333331</v>
       </c>
       <c r="AL685" s="9"/>
-      <c r="AM685" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN685" s="43" t="s">
         <v>334</v>
       </c>
@@ -80619,9 +80604,6 @@
         <v>4.1516666666666672E-3</v>
       </c>
       <c r="AL686" s="9"/>
-      <c r="AM686" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN686" s="43" t="s">
         <v>334</v>
       </c>
@@ -80755,9 +80737,6 @@
         <v>4.1516666666666672E-3</v>
       </c>
       <c r="AL687" s="9"/>
-      <c r="AM687" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN687" s="43" t="s">
         <v>334</v>
       </c>
@@ -80891,9 +80870,6 @@
         <v>0.11121947037972069</v>
       </c>
       <c r="AL688" s="9"/>
-      <c r="AM688" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN688" s="43" t="s">
         <v>334</v>
       </c>
@@ -81027,9 +81003,6 @@
         <v>0.12239480676288812</v>
       </c>
       <c r="AL689" s="9"/>
-      <c r="AM689" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN689" s="43" t="s">
         <v>334</v>
       </c>
@@ -81163,9 +81136,6 @@
         <v>4.1516666666666664E-3</v>
       </c>
       <c r="AL690" s="9"/>
-      <c r="AM690" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN690" s="43" t="s">
         <v>334</v>
       </c>
@@ -81299,9 +81269,6 @@
         <v>7.8159100246183805E-2</v>
       </c>
       <c r="AL691" s="9"/>
-      <c r="AM691" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN691" s="43" t="s">
         <v>334</v>
       </c>
@@ -81437,9 +81404,6 @@
         <f t="shared" si="439"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AM692" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN692" s="43" t="s">
         <v>334</v>
       </c>
@@ -81575,9 +81539,6 @@
         <f t="shared" si="439"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AM693" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN693" s="43" t="s">
         <v>334</v>
       </c>
@@ -81713,9 +81674,6 @@
         <f t="shared" si="439"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AM694" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN694" s="43" t="s">
         <v>334</v>
       </c>
@@ -81851,9 +81809,6 @@
         <f t="shared" si="439"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AM695" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="AN695" s="43" t="s">
         <v>334</v>
       </c>
@@ -81873,1646 +81828,6 @@
       <c r="BA695" s="45"/>
       <c r="BB695" s="47">
         <f t="shared" si="437"/>
-        <v>0.25029761904761899</v>
-      </c>
-    </row>
-    <row r="697" spans="1:54">
-      <c r="A697" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B697" s="13">
-        <v>2.2720201218169627</v>
-      </c>
-      <c r="C697" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D697" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E697" s="1">
-        <v>470</v>
-      </c>
-      <c r="F697" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G697" s="26">
-        <f t="shared" si="425"/>
-        <v>4.8340853655680057E-3</v>
-      </c>
-      <c r="K697" s="47">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="M697" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N697" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O697" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P697" s="20"/>
-      <c r="Q697" s="37"/>
-      <c r="R697" s="20">
-        <v>30</v>
-      </c>
-      <c r="S697" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T697" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U697" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V697" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W697" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X697" s="22">
-        <v>2.4</v>
-      </c>
-      <c r="Y697" s="2">
-        <f t="shared" si="429"/>
-        <v>59.783999999999999</v>
-      </c>
-      <c r="Z697" s="2">
-        <f t="shared" si="430"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="AA697" s="2">
-        <f t="shared" si="431"/>
-        <v>5.0159999999999991</v>
-      </c>
-      <c r="AB697" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC697" s="2">
-        <f t="shared" si="433"/>
-        <v>72</v>
-      </c>
-      <c r="AD697" s="13">
-        <f t="shared" si="434"/>
-        <v>4.0139022152099676E-3</v>
-      </c>
-      <c r="AE697" s="44">
-        <f>$K697*$Y697/$AC697</f>
-        <v>1.8267333333333333E-2</v>
-      </c>
-      <c r="AF697" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG697" s="5">
-        <v>2</v>
-      </c>
-      <c r="AH697" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI697" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ697" s="3">
-        <f t="shared" si="436"/>
-        <v>2.0069511076049838E-2</v>
-      </c>
-      <c r="AK697" s="47">
-        <f>$AE697*$AH697</f>
-        <v>9.1336666666666663E-2</v>
-      </c>
-      <c r="AL697" s="9"/>
-      <c r="AM697" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN697" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV697" s="45">
-        <f>(R697-S697)-V697</f>
-        <v>5.09</v>
-      </c>
-      <c r="AW697" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX697" s="45"/>
-      <c r="AY697" s="45">
-        <f>(($R697*0.25)-($S697*AW697))/(R697-S697)</f>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ697" s="45"/>
-      <c r="BA697" s="45"/>
-      <c r="BB697" s="47">
-        <f t="shared" ref="BB697:BB708" si="443">((S697*AW697)+((U697/(U697+T697))*(U697+T697))+(V697*0.25))/R697</f>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="698" spans="1:54">
-      <c r="A698" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="B698" s="13">
-        <v>2.2570557217583938</v>
-      </c>
-      <c r="C698" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D698" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E698" s="1">
-        <v>470</v>
-      </c>
-      <c r="F698" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G698" s="26">
-        <f t="shared" si="425"/>
-        <v>4.8022462165072206E-3</v>
-      </c>
-      <c r="K698" s="47">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="M698" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N698" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O698" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P698" s="20"/>
-      <c r="Q698" s="37"/>
-      <c r="R698" s="20">
-        <v>30</v>
-      </c>
-      <c r="S698" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T698" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U698" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V698" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W698" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X698" s="22">
-        <v>2.4</v>
-      </c>
-      <c r="Y698" s="2">
-        <f t="shared" si="429"/>
-        <v>59.783999999999999</v>
-      </c>
-      <c r="Z698" s="2">
-        <f t="shared" si="430"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="AA698" s="2">
-        <f t="shared" si="431"/>
-        <v>5.0159999999999991</v>
-      </c>
-      <c r="AB698" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC698" s="2">
-        <f t="shared" si="433"/>
-        <v>72</v>
-      </c>
-      <c r="AD698" s="13">
-        <f t="shared" si="434"/>
-        <v>3.9874651084398291E-3</v>
-      </c>
-      <c r="AE698" s="44">
-        <f t="shared" ref="AE698:AE708" si="444">$K698*$Y698/$AC698</f>
-        <v>5.3971666666666668E-2</v>
-      </c>
-      <c r="AF698" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG698" s="5">
-        <v>3</v>
-      </c>
-      <c r="AH698" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI698" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ698" s="3">
-        <f t="shared" si="436"/>
-        <v>1.9937325542199145E-2</v>
-      </c>
-      <c r="AK698" s="47">
-        <f t="shared" ref="AK698:AK708" si="445">$AE698*$AH698</f>
-        <v>0.26985833333333331</v>
-      </c>
-      <c r="AL698" s="9"/>
-      <c r="AM698" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN698" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV698" s="45">
-        <f t="shared" ref="AV698:AV708" si="446">(R698-S698)-V698</f>
-        <v>5.09</v>
-      </c>
-      <c r="AW698" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX698" s="45"/>
-      <c r="AY698" s="45">
-        <f t="shared" ref="AY698:AY708" si="447">(($R698*0.25)-($S698*AW698))/(R698-S698)</f>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ698" s="45"/>
-      <c r="BA698" s="45"/>
-      <c r="BB698" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="699" spans="1:54">
-      <c r="A699" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="B699" s="13">
-        <v>1.4470426381836576</v>
-      </c>
-      <c r="C699" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D699" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E699" s="1">
-        <v>470</v>
-      </c>
-      <c r="F699" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G699" s="26">
-        <f t="shared" si="425"/>
-        <v>3.0788141237950164E-3</v>
-      </c>
-      <c r="K699" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="M699" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N699" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O699" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P699" s="20"/>
-      <c r="Q699" s="37"/>
-      <c r="R699" s="20">
-        <v>30</v>
-      </c>
-      <c r="S699" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T699" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U699" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V699" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W699" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X699" s="22">
-        <v>3.4</v>
-      </c>
-      <c r="Y699" s="2">
-        <f t="shared" si="429"/>
-        <v>84.694000000000003</v>
-      </c>
-      <c r="Z699" s="2">
-        <f t="shared" si="430"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="AA699" s="2">
-        <f t="shared" si="431"/>
-        <v>7.105999999999999</v>
-      </c>
-      <c r="AB699" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC699" s="2">
-        <f t="shared" si="433"/>
-        <v>102</v>
-      </c>
-      <c r="AD699" s="13">
-        <f t="shared" si="434"/>
-        <v>2.556441994124462E-3</v>
-      </c>
-      <c r="AE699" s="44">
-        <f t="shared" si="444"/>
-        <v>8.3033333333333342E-4</v>
-      </c>
-      <c r="AF699" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG699" s="5">
-        <v>4</v>
-      </c>
-      <c r="AH699" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI699" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ699" s="3">
-        <f t="shared" si="436"/>
-        <v>1.2782209970622311E-2</v>
-      </c>
-      <c r="AK699" s="47">
-        <f t="shared" si="445"/>
-        <v>4.1516666666666672E-3</v>
-      </c>
-      <c r="AL699" s="9"/>
-      <c r="AM699" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN699" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV699" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW699" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX699" s="45"/>
-      <c r="AY699" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ699" s="45"/>
-      <c r="BA699" s="45"/>
-      <c r="BB699" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="700" spans="1:54">
-      <c r="A700" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="B700" s="13">
-        <v>1.5010077485056368</v>
-      </c>
-      <c r="C700" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D700" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E700" s="1">
-        <v>470</v>
-      </c>
-      <c r="F700" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G700" s="26">
-        <f t="shared" si="425"/>
-        <v>3.1936335074588015E-3</v>
-      </c>
-      <c r="K700" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="M700" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N700" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O700" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P700" s="20"/>
-      <c r="Q700" s="37"/>
-      <c r="R700" s="20">
-        <v>30</v>
-      </c>
-      <c r="S700" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T700" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U700" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V700" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W700" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X700" s="22">
-        <v>3.4</v>
-      </c>
-      <c r="Y700" s="2">
-        <f t="shared" si="429"/>
-        <v>84.694000000000003</v>
-      </c>
-      <c r="Z700" s="2">
-        <f t="shared" si="430"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="AA700" s="2">
-        <f t="shared" si="431"/>
-        <v>7.105999999999999</v>
-      </c>
-      <c r="AB700" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC700" s="2">
-        <f t="shared" si="433"/>
-        <v>102</v>
-      </c>
-      <c r="AD700" s="13">
-        <f t="shared" si="434"/>
-        <v>2.6517803556932915E-3</v>
-      </c>
-      <c r="AE700" s="44">
-        <f t="shared" si="444"/>
-        <v>8.3033333333333342E-4</v>
-      </c>
-      <c r="AF700" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG700" s="5">
-        <v>5</v>
-      </c>
-      <c r="AH700" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI700" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ700" s="3">
-        <f t="shared" si="436"/>
-        <v>1.3258901778466458E-2</v>
-      </c>
-      <c r="AK700" s="47">
-        <f t="shared" si="445"/>
-        <v>4.1516666666666672E-3</v>
-      </c>
-      <c r="AL700" s="9"/>
-      <c r="AM700" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN700" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV700" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW700" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX700" s="45"/>
-      <c r="AY700" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ700" s="45"/>
-      <c r="BA700" s="45"/>
-      <c r="BB700" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="701" spans="1:54">
-      <c r="A701" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="B701" s="13">
-        <v>1.9388368658222819</v>
-      </c>
-      <c r="C701" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D701" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E701" s="1">
-        <v>470</v>
-      </c>
-      <c r="F701" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G701" s="26">
-        <f t="shared" si="425"/>
-        <v>4.1251848208984721E-3</v>
-      </c>
-      <c r="K701" s="47">
-        <v>2.67891137004546E-2</v>
-      </c>
-      <c r="M701" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N701" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O701" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P701" s="20"/>
-      <c r="Q701" s="37"/>
-      <c r="R701" s="20">
-        <v>30</v>
-      </c>
-      <c r="S701" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T701" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U701" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V701" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W701" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X701" s="22">
-        <v>3.4</v>
-      </c>
-      <c r="Y701" s="2">
-        <f t="shared" si="429"/>
-        <v>84.694000000000003</v>
-      </c>
-      <c r="Z701" s="2">
-        <f t="shared" si="430"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="AA701" s="2">
-        <f t="shared" si="431"/>
-        <v>7.105999999999999</v>
-      </c>
-      <c r="AB701" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC701" s="2">
-        <f t="shared" si="433"/>
-        <v>102</v>
-      </c>
-      <c r="AD701" s="13">
-        <f t="shared" si="434"/>
-        <v>3.4252784629526978E-3</v>
-      </c>
-      <c r="AE701" s="44">
-        <f t="shared" si="444"/>
-        <v>2.2243894075944137E-2</v>
-      </c>
-      <c r="AF701" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG701" s="5">
-        <v>6</v>
-      </c>
-      <c r="AH701" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI701" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ701" s="3">
-        <f t="shared" si="436"/>
-        <v>1.712639231476349E-2</v>
-      </c>
-      <c r="AK701" s="47">
-        <f t="shared" si="445"/>
-        <v>0.11121947037972069</v>
-      </c>
-      <c r="AL701" s="9"/>
-      <c r="AM701" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN701" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV701" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW701" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX701" s="45"/>
-      <c r="AY701" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ701" s="45"/>
-      <c r="BA701" s="45"/>
-      <c r="BB701" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="702" spans="1:54">
-      <c r="A702" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="B702" s="13">
-        <v>2.0563654384731715</v>
-      </c>
-      <c r="C702" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D702" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E702" s="1">
-        <v>470</v>
-      </c>
-      <c r="F702" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G702" s="26">
-        <f t="shared" si="425"/>
-        <v>4.3752456137727052E-3</v>
-      </c>
-      <c r="K702" s="47">
-        <v>2.9480884808403399E-2</v>
-      </c>
-      <c r="M702" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N702" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O702" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P702" s="20"/>
-      <c r="Q702" s="37"/>
-      <c r="R702" s="20">
-        <v>30</v>
-      </c>
-      <c r="S702" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T702" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U702" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V702" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W702" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X702" s="22">
-        <v>3.4</v>
-      </c>
-      <c r="Y702" s="2">
-        <f t="shared" si="429"/>
-        <v>84.694000000000003</v>
-      </c>
-      <c r="Z702" s="2">
-        <f t="shared" si="430"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="AA702" s="2">
-        <f t="shared" si="431"/>
-        <v>7.105999999999999</v>
-      </c>
-      <c r="AB702" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC702" s="2">
-        <f t="shared" si="433"/>
-        <v>102</v>
-      </c>
-      <c r="AD702" s="13">
-        <f t="shared" si="434"/>
-        <v>3.6329122746359362E-3</v>
-      </c>
-      <c r="AE702" s="44">
-        <f t="shared" si="444"/>
-        <v>2.4478961352577624E-2</v>
-      </c>
-      <c r="AF702" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG702" s="5">
-        <v>7</v>
-      </c>
-      <c r="AH702" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI702" s="2">
-        <f t="shared" si="435"/>
-        <v>4.1516666666666664</v>
-      </c>
-      <c r="AJ702" s="3">
-        <f t="shared" si="436"/>
-        <v>1.8164561373179681E-2</v>
-      </c>
-      <c r="AK702" s="47">
-        <f t="shared" si="445"/>
-        <v>0.12239480676288812</v>
-      </c>
-      <c r="AL702" s="9"/>
-      <c r="AM702" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN702" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV702" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW702" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX702" s="45"/>
-      <c r="AY702" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ702" s="45"/>
-      <c r="BA702" s="45"/>
-      <c r="BB702" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="703" spans="1:54">
-      <c r="A703" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="B703" s="13">
-        <v>2.8624641505678192</v>
-      </c>
-      <c r="C703" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D703" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E703" s="1">
-        <v>470</v>
-      </c>
-      <c r="F703" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G703" s="26">
-        <f t="shared" si="425"/>
-        <v>6.0903492565272752E-3</v>
-      </c>
-      <c r="K703" s="47">
-        <v>1E-3</v>
-      </c>
-      <c r="M703" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N703" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O703" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P703" s="20"/>
-      <c r="Q703" s="37"/>
-      <c r="R703" s="20">
-        <v>30</v>
-      </c>
-      <c r="S703" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T703" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U703" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V703" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W703" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X703" s="22">
-        <v>2.5</v>
-      </c>
-      <c r="Y703" s="2">
-        <f t="shared" si="429"/>
-        <v>62.274999999999999</v>
-      </c>
-      <c r="Z703" s="2">
-        <f t="shared" si="430"/>
-        <v>7.5</v>
-      </c>
-      <c r="AA703" s="2">
-        <f t="shared" si="431"/>
-        <v>5.2249999999999996</v>
-      </c>
-      <c r="AB703" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC703" s="2">
-        <f t="shared" si="433"/>
-        <v>75</v>
-      </c>
-      <c r="AD703" s="13">
-        <f t="shared" si="434"/>
-        <v>5.057019999336481E-3</v>
-      </c>
-      <c r="AE703" s="44">
-        <f t="shared" si="444"/>
-        <v>8.3033333333333331E-4</v>
-      </c>
-      <c r="AF703" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG703" s="5">
-        <v>8</v>
-      </c>
-      <c r="AH703" s="20">
-        <v>2.5</v>
-      </c>
-      <c r="AI703" s="2">
-        <f t="shared" si="435"/>
-        <v>2.0758333333333332</v>
-      </c>
-      <c r="AJ703" s="3">
-        <f t="shared" si="436"/>
-        <v>1.2642549998341203E-2</v>
-      </c>
-      <c r="AK703" s="47">
-        <f t="shared" si="445"/>
-        <v>2.0758333333333332E-3</v>
-      </c>
-      <c r="AL703" s="9"/>
-      <c r="AM703" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN703" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV703" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW703" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX703" s="45"/>
-      <c r="AY703" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ703" s="45"/>
-      <c r="BA703" s="45"/>
-      <c r="BB703" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="704" spans="1:54">
-      <c r="A704" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="B704" s="13">
-        <v>2.7495590340357059</v>
-      </c>
-      <c r="C704" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D704" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E704" s="1">
-        <v>470</v>
-      </c>
-      <c r="F704" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G704" s="26">
-        <f t="shared" si="425"/>
-        <v>5.8501256043312893E-3</v>
-      </c>
-      <c r="K704" s="47">
-        <v>1.8825957506106099E-2</v>
-      </c>
-      <c r="M704" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N704" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O704" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P704" s="20"/>
-      <c r="Q704" s="37"/>
-      <c r="R704" s="20">
-        <v>30</v>
-      </c>
-      <c r="S704" s="2">
-        <v>24.91</v>
-      </c>
-      <c r="T704" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U704" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="V704" s="2">
-        <f t="shared" si="427"/>
-        <v>0</v>
-      </c>
-      <c r="W704" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X704" s="22">
-        <v>2.5</v>
-      </c>
-      <c r="Y704" s="2">
-        <f t="shared" si="429"/>
-        <v>62.274999999999999</v>
-      </c>
-      <c r="Z704" s="2">
-        <f t="shared" si="430"/>
-        <v>7.5</v>
-      </c>
-      <c r="AA704" s="2">
-        <f t="shared" si="431"/>
-        <v>5.2249999999999996</v>
-      </c>
-      <c r="AB704" s="2">
-        <f t="shared" si="432"/>
-        <v>0</v>
-      </c>
-      <c r="AC704" s="2">
-        <f t="shared" si="433"/>
-        <v>75</v>
-      </c>
-      <c r="AD704" s="13">
-        <f t="shared" si="434"/>
-        <v>4.8575542934630811E-3</v>
-      </c>
-      <c r="AE704" s="44">
-        <f t="shared" si="444"/>
-        <v>1.5631820049236762E-2</v>
-      </c>
-      <c r="AF704" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG704" s="5">
-        <v>9</v>
-      </c>
-      <c r="AH704" s="20">
-        <v>4</v>
-      </c>
-      <c r="AI704" s="2">
-        <f t="shared" si="435"/>
-        <v>3.3213333333333335</v>
-      </c>
-      <c r="AJ704" s="3">
-        <f t="shared" si="436"/>
-        <v>1.9430217173852325E-2</v>
-      </c>
-      <c r="AK704" s="47">
-        <f t="shared" si="445"/>
-        <v>6.2527280196947047E-2</v>
-      </c>
-      <c r="AL704" s="9"/>
-      <c r="AM704" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN704" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV704" s="45">
-        <f t="shared" si="446"/>
-        <v>5.09</v>
-      </c>
-      <c r="AW704" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX704" s="45"/>
-      <c r="AY704" s="45">
-        <f t="shared" si="447"/>
-        <v>0.41149901768172886</v>
-      </c>
-      <c r="AZ704" s="45"/>
-      <c r="BA704" s="45"/>
-      <c r="BB704" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24984900000000002</v>
-      </c>
-    </row>
-    <row r="705" spans="1:54">
-      <c r="A705" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="B705" s="13">
-        <v>1.8673339618529914</v>
-      </c>
-      <c r="C705" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D705" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E705" s="1">
-        <v>470</v>
-      </c>
-      <c r="F705" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G705" s="26">
-        <f t="shared" si="425"/>
-        <v>3.9730509826659387E-3</v>
-      </c>
-      <c r="K705" s="47">
-        <v>0.12978674428932899</v>
-      </c>
-      <c r="M705" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N705" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O705" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P705" s="20"/>
-      <c r="Q705" s="37">
-        <v>2</v>
-      </c>
-      <c r="R705" s="20">
-        <v>30</v>
-      </c>
-      <c r="S705" s="2">
-        <f t="shared" ref="S705:S708" si="448">($Q705/$K705)</f>
-        <v>15.409894214939786</v>
-      </c>
-      <c r="T705" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U705" s="2">
-        <v>1.67</v>
-      </c>
-      <c r="V705" s="2">
-        <f t="shared" si="427"/>
-        <v>9.9201057850602155</v>
-      </c>
-      <c r="W705" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X705" s="22">
-        <v>3.7</v>
-      </c>
-      <c r="Y705" s="2">
-        <f t="shared" si="429"/>
-        <v>57.016608595277212</v>
-      </c>
-      <c r="Z705" s="2">
-        <f t="shared" si="430"/>
-        <v>11.100000000000001</v>
-      </c>
-      <c r="AA705" s="2">
-        <f t="shared" si="431"/>
-        <v>6.1790000000000003</v>
-      </c>
-      <c r="AB705" s="2">
-        <f t="shared" si="432"/>
-        <v>36.704391404722799</v>
-      </c>
-      <c r="AC705" s="2">
-        <f t="shared" si="433"/>
-        <v>111.00000000000001</v>
-      </c>
-      <c r="AD705" s="13">
-        <f t="shared" si="434"/>
-        <v>2.0408098451148225E-3</v>
-      </c>
-      <c r="AE705" s="44">
-        <f t="shared" si="444"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="AF705" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG705" s="5">
-        <v>10</v>
-      </c>
-      <c r="AH705" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI705" s="2">
-        <f t="shared" si="435"/>
-        <v>2.5683157024899641</v>
-      </c>
-      <c r="AJ705" s="3">
-        <f t="shared" si="436"/>
-        <v>1.0204049225574113E-2</v>
-      </c>
-      <c r="AK705" s="47">
-        <f t="shared" si="445"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AM705" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN705" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV705" s="45">
-        <f t="shared" si="446"/>
-        <v>4.6699999999999982</v>
-      </c>
-      <c r="AW705" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX705" s="45"/>
-      <c r="AY705" s="45">
-        <f t="shared" si="447"/>
-        <v>0.28485420301844055</v>
-      </c>
-      <c r="AZ705" s="45"/>
-      <c r="BA705" s="45"/>
-      <c r="BB705" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24979911636356625</v>
-      </c>
-    </row>
-    <row r="706" spans="1:54">
-      <c r="A706" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="B706" s="13">
-        <v>1.879438092483444</v>
-      </c>
-      <c r="C706" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D706" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E706" s="1">
-        <v>470</v>
-      </c>
-      <c r="F706" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G706" s="26">
-        <f t="shared" si="425"/>
-        <v>3.9988044520924337E-3</v>
-      </c>
-      <c r="K706" s="47">
-        <v>0.101727466721955</v>
-      </c>
-      <c r="M706" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N706" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O706" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P706" s="20"/>
-      <c r="Q706" s="37">
-        <v>2</v>
-      </c>
-      <c r="R706" s="20">
-        <v>30</v>
-      </c>
-      <c r="S706" s="2">
-        <f t="shared" si="448"/>
-        <v>19.660373588840745</v>
-      </c>
-      <c r="T706" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U706" s="2">
-        <v>1.85</v>
-      </c>
-      <c r="V706" s="2">
-        <f t="shared" si="427"/>
-        <v>5.4896264111592536</v>
-      </c>
-      <c r="W706" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X706" s="22">
-        <v>3</v>
-      </c>
-      <c r="Y706" s="2">
-        <f t="shared" si="429"/>
-        <v>58.981120766522238</v>
-      </c>
-      <c r="Z706" s="2">
-        <f t="shared" si="430"/>
-        <v>9</v>
-      </c>
-      <c r="AA706" s="2">
-        <f t="shared" si="431"/>
-        <v>5.5500000000000007</v>
-      </c>
-      <c r="AB706" s="2">
-        <f t="shared" si="432"/>
-        <v>16.468879233477761</v>
-      </c>
-      <c r="AC706" s="2">
-        <f t="shared" si="433"/>
-        <v>90</v>
-      </c>
-      <c r="AD706" s="13">
-        <f t="shared" si="434"/>
-        <v>2.6205996478952292E-3</v>
-      </c>
-      <c r="AE706" s="44">
-        <f t="shared" si="444"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="AF706" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG706" s="5">
-        <v>11</v>
-      </c>
-      <c r="AH706" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI706" s="2">
-        <f t="shared" si="435"/>
-        <v>3.2767289314734573</v>
-      </c>
-      <c r="AJ706" s="3">
-        <f t="shared" si="436"/>
-        <v>1.3102998239476145E-2</v>
-      </c>
-      <c r="AK706" s="47">
-        <f t="shared" si="445"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AM706" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN706" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV706" s="45">
-        <f t="shared" si="446"/>
-        <v>4.8500000000000014</v>
-      </c>
-      <c r="AW706" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX706" s="45"/>
-      <c r="AY706" s="45">
-        <f t="shared" si="447"/>
-        <v>0.31274814027434511</v>
-      </c>
-      <c r="AZ706" s="45"/>
-      <c r="BA706" s="45"/>
-      <c r="BB706" s="47">
-        <f t="shared" si="443"/>
-        <v>0.24962358905227519</v>
-      </c>
-    </row>
-    <row r="707" spans="1:54">
-      <c r="A707" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="B707" s="13">
-        <v>2.4080610097494177</v>
-      </c>
-      <c r="C707" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D707" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E707" s="1">
-        <v>470</v>
-      </c>
-      <c r="F707" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G707" s="26">
-        <f t="shared" si="425"/>
-        <v>5.1235340632966335E-3</v>
-      </c>
-      <c r="K707" s="47">
-        <v>0.110858079193025</v>
-      </c>
-      <c r="M707" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N707" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O707" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P707" s="20"/>
-      <c r="Q707" s="37">
-        <v>2</v>
-      </c>
-      <c r="R707" s="20">
-        <v>30</v>
-      </c>
-      <c r="S707" s="2">
-        <f t="shared" si="448"/>
-        <v>18.041084732467894</v>
-      </c>
-      <c r="T707" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U707" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="V707" s="2">
-        <f t="shared" si="427"/>
-        <v>7.1589152675321053</v>
-      </c>
-      <c r="W707" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X707" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="Y707" s="2">
-        <f t="shared" si="429"/>
-        <v>27.061627098701841</v>
-      </c>
-      <c r="Z707" s="2">
-        <f t="shared" si="430"/>
-        <v>4.5</v>
-      </c>
-      <c r="AA707" s="2">
-        <f t="shared" si="431"/>
-        <v>2.7</v>
-      </c>
-      <c r="AB707" s="2">
-        <f t="shared" si="432"/>
-        <v>10.738372901298158</v>
-      </c>
-      <c r="AC707" s="2">
-        <f t="shared" si="433"/>
-        <v>45</v>
-      </c>
-      <c r="AD707" s="13">
-        <f t="shared" si="434"/>
-        <v>3.0811370721873363E-3</v>
-      </c>
-      <c r="AE707" s="44">
-        <f t="shared" si="444"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="AF707" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG707" s="5">
-        <v>12</v>
-      </c>
-      <c r="AH707" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI707" s="2">
-        <f t="shared" si="435"/>
-        <v>3.0068474554113154</v>
-      </c>
-      <c r="AJ707" s="3">
-        <f t="shared" si="436"/>
-        <v>1.5405685360936682E-2</v>
-      </c>
-      <c r="AK707" s="47">
-        <f t="shared" si="445"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AM707" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN707" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV707" s="45">
-        <f t="shared" si="446"/>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="AW707" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX707" s="45"/>
-      <c r="AY707" s="45">
-        <f t="shared" si="447"/>
-        <v>0.29978342791572438</v>
-      </c>
-      <c r="AZ707" s="45"/>
-      <c r="BA707" s="45"/>
-      <c r="BB707" s="47">
-        <f t="shared" si="443"/>
-        <v>0.25015480679428531</v>
-      </c>
-    </row>
-    <row r="708" spans="1:54">
-      <c r="A708" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="B708" s="13">
-        <v>2.4191921198213535</v>
-      </c>
-      <c r="C708" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D708" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E708" s="1">
-        <v>470</v>
-      </c>
-      <c r="F708" s="29">
-        <v>44014</v>
-      </c>
-      <c r="G708" s="26">
-        <f t="shared" si="425"/>
-        <v>5.1472172762156458E-3</v>
-      </c>
-      <c r="K708" s="47">
-        <v>0.105</v>
-      </c>
-      <c r="M708" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="N708" s="7">
-        <v>44026</v>
-      </c>
-      <c r="O708" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P708" s="20"/>
-      <c r="Q708" s="37">
-        <v>2</v>
-      </c>
-      <c r="R708" s="20">
-        <v>30</v>
-      </c>
-      <c r="S708" s="2">
-        <f t="shared" si="448"/>
-        <v>19.047619047619047</v>
-      </c>
-      <c r="T708" s="2">
-        <f t="shared" si="426"/>
-        <v>3</v>
-      </c>
-      <c r="U708" s="2">
-        <v>1.85</v>
-      </c>
-      <c r="V708" s="2">
-        <f t="shared" si="427"/>
-        <v>6.1023809523809511</v>
-      </c>
-      <c r="W708" s="5">
-        <f t="shared" si="428"/>
-        <v>30</v>
-      </c>
-      <c r="X708" s="22">
-        <v>1.45</v>
-      </c>
-      <c r="Y708" s="2">
-        <f t="shared" si="429"/>
-        <v>27.619047619047617</v>
-      </c>
-      <c r="Z708" s="2">
-        <f t="shared" si="430"/>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="AA708" s="2">
-        <f t="shared" si="431"/>
-        <v>2.6825000000000001</v>
-      </c>
-      <c r="AB708" s="2">
-        <f t="shared" si="432"/>
-        <v>8.848452380952379</v>
-      </c>
-      <c r="AC708" s="2">
-        <f t="shared" si="433"/>
-        <v>43.499999999999993</v>
-      </c>
-      <c r="AD708" s="13">
-        <f t="shared" si="434"/>
-        <v>3.2680744610892988E-3</v>
-      </c>
-      <c r="AE708" s="44">
-        <f t="shared" si="444"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="AF708" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG708" s="5">
-        <v>13</v>
-      </c>
-      <c r="AH708" s="20">
-        <v>5</v>
-      </c>
-      <c r="AI708" s="2">
-        <f t="shared" si="435"/>
-        <v>3.1746031746031749</v>
-      </c>
-      <c r="AJ708" s="3">
-        <f t="shared" si="436"/>
-        <v>1.6340372305446493E-2</v>
-      </c>
-      <c r="AK708" s="47">
-        <f t="shared" si="445"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AM708" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN708" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV708" s="45">
-        <f t="shared" si="446"/>
-        <v>4.8500000000000014</v>
-      </c>
-      <c r="AW708" s="43">
-        <v>0.217</v>
-      </c>
-      <c r="AX708" s="45"/>
-      <c r="AY708" s="45">
-        <f t="shared" si="447"/>
-        <v>0.30739130434782613</v>
-      </c>
-      <c r="AZ708" s="45"/>
-      <c r="BA708" s="45"/>
-      <c r="BB708" s="47">
-        <f t="shared" si="443"/>
         <v>0.25029761904761899</v>
       </c>
     </row>

</xml_diff>